<commit_message>
Reports / case counts DONE
</commit_message>
<xml_diff>
--- a/src/JCSGYK/AdminBundle/Resources/public/reports/casecounts.xlsx
+++ b/src/JCSGYK/AdminBundle/Resources/public/reports/casecounts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Név</t>
   </si>
@@ -27,34 +27,34 @@
     <t>Józsefvárosi Szociális Szolgáltató és Gyermekjóléti központ</t>
   </si>
   <si>
-    <t>Készült:</t>
-  </si>
-  <si>
-    <t>[sp.datum]</t>
-  </si>
-  <si>
-    <t>[admin.nev;block=tbs:row]</t>
-  </si>
-  <si>
     <t>Összes eset</t>
   </si>
   <si>
-    <t>[admin.total]</t>
-  </si>
-  <si>
     <t>Aktív</t>
   </si>
   <si>
     <t>Lezárt</t>
   </si>
   <si>
-    <t>[admin.active]</t>
-  </si>
-  <si>
-    <t>[admin.archived]</t>
-  </si>
-  <si>
     <t>Esetszám kimutatás</t>
+  </si>
+  <si>
+    <t>[casecount.lastname;block=tbs:row] [casecount.firstname]</t>
+  </si>
+  <si>
+    <t>Készült: [sp.datum]</t>
+  </si>
+  <si>
+    <t>[casecount.enabled;if [val]=0;then '';else 'x']</t>
+  </si>
+  <si>
+    <t>[casecount.total;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[casecount.active;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[casecount.archived;ope=tbs:num]</t>
   </si>
 </sst>
 </file>
@@ -129,7 +129,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -139,23 +139,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -553,74 +558,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="7" width="8.83203125" customWidth="1"/>
-    <col min="9" max="15" width="8.83203125" customWidth="1"/>
+    <col min="2" max="2" width="4.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="8" width="8.83203125" customWidth="1"/>
+    <col min="10" max="16" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1">
+    <row r="6" spans="1:10" s="2" customFormat="1">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:9" s="4" customFormat="1">
+    <row r="7" spans="1:10" s="4" customFormat="1">
       <c r="A7" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>